<commit_message>
all changes 1707: button, infeed and so on
</commit_message>
<xml_diff>
--- a/layout.xlsx
+++ b/layout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\STM32\projects_link\p5encoder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\STM32\project\efeed\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -78,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I20" authorId="0" shapeId="0">
+    <comment ref="I21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J20" authorId="0" shapeId="0">
+    <comment ref="J21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -126,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K20" authorId="0" shapeId="0">
+    <comment ref="K21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -151,7 +151,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L20" authorId="0" shapeId="0">
+    <comment ref="L21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -175,7 +175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R20" authorId="0" shapeId="0">
+    <comment ref="R21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -200,7 +200,202 @@
         </r>
       </text>
     </comment>
-    <comment ref="S20" authorId="0" shapeId="0">
+    <comment ref="S21" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sergey Taranov:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+T4_CH2
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O42" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sergey Taranov:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+T2_CH2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P42" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sergey Taranov:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+T2_CH1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E48" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sergey Taranov:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+T1_CH1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F48" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sergey Taranov:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+T1_CH2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G48" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sergey Taranov:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+T1_CH3
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H48" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sergey Taranov:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+T1_CH4</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N48" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sergey Taranov:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+T4_CH1
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O48" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -230,7 +425,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="61">
   <si>
     <t>B11</t>
   </si>
@@ -404,6 +599,15 @@
   </si>
   <si>
     <t>servo1</t>
+  </si>
+  <si>
+    <t>+32</t>
+  </si>
+  <si>
+    <t>+16</t>
+  </si>
+  <si>
+    <t>+5</t>
   </si>
 </sst>
 </file>
@@ -433,12 +637,42 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -505,7 +739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -519,6 +753,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -528,8 +768,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -909,10 +1173,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB23"/>
+  <dimension ref="A1:AB50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W25" sqref="W25"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AA35" sqref="AA35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1044,76 +1308,76 @@
     <row r="10" spans="1:28" ht="15.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:28" ht="15.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="1:28" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E12" s="8">
+      <c r="E12" s="5">
         <v>1</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="5">
         <v>2</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="5">
         <v>3</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="5">
         <v>4</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="5">
         <v>5</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="5">
         <v>6</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K12" s="5">
         <v>7</v>
       </c>
-      <c r="L12" s="8">
+      <c r="L12" s="5">
         <v>8</v>
       </c>
-      <c r="M12" s="8">
+      <c r="M12" s="5">
         <v>9</v>
       </c>
-      <c r="N12" s="8">
+      <c r="N12" s="5">
         <v>10</v>
       </c>
-      <c r="O12" s="8">
+      <c r="O12" s="5">
         <v>11</v>
       </c>
-      <c r="P12" s="8">
+      <c r="P12" s="5">
         <v>12</v>
       </c>
-      <c r="Q12" s="8">
+      <c r="Q12" s="5">
         <v>13</v>
       </c>
-      <c r="R12" s="8">
+      <c r="R12" s="5">
         <v>14</v>
       </c>
-      <c r="S12" s="8">
+      <c r="S12" s="5">
         <v>15</v>
       </c>
-      <c r="T12" s="8">
+      <c r="T12" s="5">
         <v>16</v>
       </c>
-      <c r="U12" s="8">
+      <c r="U12" s="5">
         <v>17</v>
       </c>
-      <c r="V12" s="8">
+      <c r="V12" s="5">
         <v>18</v>
       </c>
-      <c r="W12" s="8">
+      <c r="W12" s="5">
         <v>19</v>
       </c>
-      <c r="X12" s="8">
+      <c r="X12" s="5">
         <v>20</v>
       </c>
-      <c r="Y12" s="8">
+      <c r="Y12" s="5">
         <v>21</v>
       </c>
-      <c r="Z12" s="8">
+      <c r="Z12" s="5">
         <v>22</v>
       </c>
-      <c r="AA12" s="8">
+      <c r="AA12" s="5">
         <v>23</v>
       </c>
-      <c r="AB12" s="8">
+      <c r="AB12" s="5">
         <v>24</v>
       </c>
     </row>
@@ -1122,15 +1386,15 @@
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="J14" s="4"/>
-      <c r="P14" s="5" t="s">
+      <c r="J14" s="6"/>
+      <c r="P14" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="C15">
@@ -1221,71 +1485,71 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="3:24" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:24" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C17">
         <v>4</v>
       </c>
       <c r="E17" s="2"/>
+      <c r="F17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="X17" s="2"/>
     </row>
-    <row r="18" spans="3:24" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:24" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C18">
         <v>5</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U18" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
     </row>
-    <row r="19" spans="3:24" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:24" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C19">
         <v>6</v>
       </c>
@@ -1310,91 +1574,91 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
+      <c r="R19" t="s">
+        <v>46</v>
+      </c>
+      <c r="S19" t="s">
+        <v>47</v>
+      </c>
+      <c r="T19" t="s">
+        <v>48</v>
+      </c>
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
     </row>
-    <row r="20" spans="3:24" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="C20">
         <v>7</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T20" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="U20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="V20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="W20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X20" s="1">
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="21" spans="3:24" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:24" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C21">
         <v>8</v>
       </c>
-      <c r="R21" t="s">
-        <v>46</v>
-      </c>
-      <c r="S21" t="s">
-        <v>47</v>
-      </c>
-      <c r="T21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="3:24" x14ac:dyDescent="0.35">
+      <c r="E21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X21" s="1">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="C22">
         <v>9</v>
       </c>
@@ -1447,33 +1711,819 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="3:24" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
       <c r="C23">
         <v>10</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="H23" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="7"/>
-      <c r="P23" s="6" t="s">
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="9"/>
+      <c r="P23" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="9"/>
+    </row>
+    <row r="31" spans="1:24" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="5">
+        <v>1</v>
+      </c>
+      <c r="B31" s="5">
+        <v>2</v>
+      </c>
+      <c r="C31" s="5">
+        <v>3</v>
+      </c>
+      <c r="D31" s="5">
+        <v>4</v>
+      </c>
+      <c r="E31" s="5">
+        <v>5</v>
+      </c>
+      <c r="F31" s="5">
+        <v>6</v>
+      </c>
+      <c r="G31" s="5">
+        <v>7</v>
+      </c>
+      <c r="H31" s="5">
+        <v>8</v>
+      </c>
+      <c r="I31" s="5">
+        <v>9</v>
+      </c>
+      <c r="J31" s="5">
+        <v>10</v>
+      </c>
+      <c r="K31" s="5">
+        <v>11</v>
+      </c>
+      <c r="L31" s="5">
+        <v>12</v>
+      </c>
+      <c r="M31" s="5">
+        <v>13</v>
+      </c>
+      <c r="N31" s="5">
+        <v>14</v>
+      </c>
+      <c r="O31" s="5">
+        <v>15</v>
+      </c>
+      <c r="P31" s="5">
+        <v>16</v>
+      </c>
+      <c r="Q31" s="5">
+        <v>17</v>
+      </c>
+      <c r="R31" s="5">
+        <v>18</v>
+      </c>
+      <c r="S31" s="5">
+        <v>19</v>
+      </c>
+      <c r="T31" s="5">
+        <v>20</v>
+      </c>
+      <c r="U31" s="5">
+        <v>21</v>
+      </c>
+      <c r="V31" s="5">
+        <v>22</v>
+      </c>
+      <c r="W31" s="5">
+        <v>23</v>
+      </c>
+      <c r="X31" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="21.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="2"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+      <c r="Y33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="2"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="K34" s="10"/>
+      <c r="L34" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="2"/>
+      <c r="Y34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="2"/>
+      <c r="B35" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="J35" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K35" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q35" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="R35" s="10"/>
+      <c r="S35" s="10"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+      <c r="X35" s="2"/>
+      <c r="Y35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="12"/>
+      <c r="P36" s="12"/>
+      <c r="Q36" s="12"/>
+      <c r="R36" s="12"/>
+      <c r="S36" s="10"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2"/>
+      <c r="W36" s="2"/>
+      <c r="X36" s="2"/>
+      <c r="Y36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="10"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="12"/>
+      <c r="S37" s="10"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+      <c r="V37" s="2"/>
+      <c r="W37" s="2"/>
+      <c r="X37" s="2"/>
+      <c r="Y37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="10"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="12"/>
+      <c r="S38" s="10"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
+      <c r="V38" s="2"/>
+      <c r="W38" s="2"/>
+      <c r="X38" s="2"/>
+      <c r="Y38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="10"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="12"/>
+      <c r="S39" s="10"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
+      <c r="V39" s="2"/>
+      <c r="W39" s="2"/>
+      <c r="X39" s="2"/>
+      <c r="Y39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="10"/>
+      <c r="B40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L40" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O40" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q40" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R40" s="12"/>
+      <c r="S40" s="10"/>
+      <c r="T40" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="U40" s="14"/>
+      <c r="V40" s="2"/>
+      <c r="W40" s="2"/>
+      <c r="X40" s="2"/>
+      <c r="Y40">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="10"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F41" s="6"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="2"/>
+      <c r="S41" s="2"/>
+      <c r="T41" s="1"/>
+      <c r="U41" s="14"/>
+      <c r="V41" s="2"/>
+      <c r="W41" s="2"/>
+      <c r="X41" s="2"/>
+      <c r="Y41">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="P42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U42" s="14"/>
+      <c r="V42" s="2"/>
+      <c r="W42" s="2"/>
+      <c r="X42" s="2"/>
+      <c r="Y42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="P43" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
+      <c r="U43" s="14"/>
+      <c r="V43" s="2"/>
+      <c r="W43" s="2"/>
+      <c r="X43" s="2"/>
+      <c r="Y43">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="2"/>
+      <c r="S44" s="2"/>
+      <c r="T44" s="2"/>
+      <c r="U44" s="14"/>
+      <c r="V44" s="2"/>
+      <c r="W44" s="2"/>
+      <c r="X44" s="2"/>
+      <c r="Y44">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
+      <c r="R45" s="2"/>
+      <c r="S45" s="2"/>
+      <c r="T45" s="2"/>
+      <c r="U45" s="14"/>
+      <c r="V45" s="2"/>
+      <c r="W45" s="2"/>
+      <c r="X45" s="2"/>
+      <c r="Y45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+      <c r="R46" s="14"/>
+      <c r="S46" s="14"/>
+      <c r="T46" s="14"/>
+      <c r="U46" s="14"/>
+      <c r="V46" s="2"/>
+      <c r="W46" s="2"/>
+      <c r="X46" s="2"/>
+      <c r="Y46">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+      <c r="R47" s="14"/>
+      <c r="S47" s="2"/>
+      <c r="T47" s="2"/>
+      <c r="U47" s="2"/>
+      <c r="V47" s="2"/>
+      <c r="W47" s="2"/>
+      <c r="X47" s="2"/>
+      <c r="Y47">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O48" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q48" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R48" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="S48" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T48" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="U48" s="2"/>
+      <c r="V48" s="2"/>
+      <c r="W48" s="2"/>
+      <c r="X48" s="2"/>
+      <c r="Y48">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O49" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q49" s="2"/>
+      <c r="R49" s="2"/>
+      <c r="S49" s="2"/>
+      <c r="T49" s="2"/>
+      <c r="U49" s="2"/>
+      <c r="V49" s="2"/>
+      <c r="W49" s="2"/>
+      <c r="X49" s="2"/>
+      <c r="Y49">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="2"/>
+      <c r="S50" s="2"/>
+      <c r="T50" s="2"/>
+      <c r="U50" s="2"/>
+      <c r="V50" s="2"/>
+      <c r="W50" s="2"/>
+      <c r="X50" s="2"/>
+      <c r="Y50">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="L34:O34"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="E41:F41"/>
     <mergeCell ref="I14:J14"/>
     <mergeCell ref="P14:R14"/>
     <mergeCell ref="P23:S23"/>
     <mergeCell ref="H23:K23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
rename X axis to Z like in cnc, start adding support for X(crosslide) axis
</commit_message>
<xml_diff>
--- a/layout.xlsx
+++ b/layout.xlsx
@@ -425,7 +425,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="65">
   <si>
     <t>B11</t>
   </si>
@@ -607,9 +607,6 @@
     <t>+16</t>
   </si>
   <si>
-    <t>+5</t>
-  </si>
-  <si>
     <t>button</t>
   </si>
   <si>
@@ -617,13 +614,19 @@
   </si>
   <si>
     <t>bluetoooth?</t>
+  </si>
+  <si>
+    <t>○</t>
+  </si>
+  <si>
+    <t>22-23% масштаб реальный</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -660,8 +663,24 @@
       <family val="3"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -704,8 +723,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -765,11 +796,233 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -795,9 +1048,6 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -805,6 +1055,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -819,20 +1075,134 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1214,13 +1584,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P46" sqref="P46"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="V32" sqref="V32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="28" width="6.6328125" customWidth="1"/>
+    <col min="1" max="26" width="6.6328125" customWidth="1"/>
+    <col min="27" max="27" width="3.1796875" customWidth="1"/>
+    <col min="28" max="28" width="6.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.35">
@@ -1425,15 +1797,15 @@
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="J14" s="13"/>
-      <c r="P14" s="14" t="s">
+      <c r="J14" s="14"/>
+      <c r="P14" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="C15">
@@ -1754,20 +2126,30 @@
       <c r="C23">
         <v>10</v>
       </c>
-      <c r="H23" s="15" t="s">
+      <c r="H23" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="16"/>
-      <c r="P23" s="15" t="s">
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="17"/>
+      <c r="P23" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="16"/>
-    </row>
-    <row r="31" spans="1:24" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="17"/>
+    </row>
+    <row r="30" spans="1:24" ht="21" x14ac:dyDescent="0.5">
+      <c r="A30" s="60" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="60"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+    </row>
+    <row r="31" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>1</v>
       </c>
@@ -1841,23 +2223,36 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:24" ht="21.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="33" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="R32">
+        <f>16.76/2.54</f>
+        <v>6.5984251968503944</v>
+      </c>
+      <c r="S32">
+        <f>13.208/2.54</f>
+        <v>5.2</v>
+      </c>
+      <c r="U32">
+        <f>18.54/2.54</f>
+        <v>7.2992125984251963</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="2"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
       <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="23"/>
       <c r="P33" s="6"/>
       <c r="Q33" s="6"/>
       <c r="R33" s="2"/>
@@ -1871,32 +2266,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:25" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="2"/>
       <c r="B34" s="7"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="18" t="s">
+      <c r="D34" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="8" t="s">
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="I34" s="6" t="s">
+      <c r="I34" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="J34" s="7" t="s">
+      <c r="J34" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="K34" s="6"/>
-      <c r="L34" s="18" t="s">
+      <c r="K34" s="26"/>
+      <c r="L34" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="M34" s="17"/>
-      <c r="N34" s="17"/>
-      <c r="O34" s="19"/>
+      <c r="M34" s="21"/>
+      <c r="N34" s="21"/>
+      <c r="O34" s="22"/>
       <c r="P34" s="2"/>
       <c r="Q34" s="6"/>
       <c r="R34" s="2"/>
@@ -1910,7 +2305,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:25" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
       <c r="B35" s="7" t="s">
         <v>36</v>
@@ -1918,43 +2313,43 @@
       <c r="C35" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F35" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G35" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="H35" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="I35" s="6" t="s">
+      <c r="I35" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="J35" s="7" t="s">
+      <c r="J35" s="29" t="s">
         <v>36</v>
       </c>
       <c r="K35" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="L35" s="1" t="s">
+      <c r="L35" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="M35" s="1" t="s">
+      <c r="M35" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="N35" s="1" t="s">
+      <c r="N35" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="O35" s="1" t="s">
+      <c r="O35" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="P35" s="1" t="s">
+      <c r="P35" s="13" t="s">
         <v>38</v>
       </c>
       <c r="Q35" s="6" t="s">
@@ -1971,7 +2366,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:25" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -1987,9 +2382,9 @@
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
       <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
       <c r="S36" s="6"/>
       <c r="T36" s="2"/>
       <c r="U36" s="2"/>
@@ -2000,7 +2395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:25" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="6"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -2015,11 +2410,11 @@
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
+      <c r="O37" s="40"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
-      <c r="R37" s="8"/>
-      <c r="S37" s="6"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="23"/>
       <c r="T37" s="2"/>
       <c r="U37" s="2"/>
       <c r="V37" s="2"/>
@@ -2029,7 +2424,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:25" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="6"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2044,11 +2439,15 @@
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
-      <c r="O38" s="2"/>
-      <c r="P38" s="2"/>
-      <c r="Q38" s="2"/>
-      <c r="R38" s="8"/>
-      <c r="S38" s="6"/>
+      <c r="O38" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="P38" s="41"/>
+      <c r="Q38" s="41"/>
+      <c r="R38" s="41"/>
+      <c r="S38" s="54" t="s">
+        <v>63</v>
+      </c>
       <c r="T38" s="2"/>
       <c r="U38" s="2"/>
       <c r="V38" s="2"/>
@@ -2058,26 +2457,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:25" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="6"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
-      <c r="L39" s="12"/>
-      <c r="M39" s="12"/>
-      <c r="N39" s="12"/>
-      <c r="O39" s="12"/>
-      <c r="P39" s="2"/>
-      <c r="Q39" s="2"/>
-      <c r="R39" s="8"/>
-      <c r="S39" s="6"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11"/>
+      <c r="O39" s="44"/>
+      <c r="P39" s="43"/>
+      <c r="Q39" s="43"/>
+      <c r="R39" s="43"/>
+      <c r="S39" s="48"/>
       <c r="T39" s="2"/>
       <c r="U39" s="2"/>
       <c r="V39" s="2"/>
@@ -2087,24 +2486,24 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:25" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="6"/>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D40" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F40" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="G40" s="11" t="s">
+      <c r="G40" s="10" t="s">
         <v>43</v>
       </c>
       <c r="H40" s="1" t="s">
@@ -2113,22 +2512,22 @@
       <c r="I40" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="J40" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="K40" s="1" t="s">
+      <c r="K40" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="L40" s="11" t="s">
+      <c r="L40" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="M40" s="1" t="s">
+      <c r="M40" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="N40" s="1" t="s">
+      <c r="N40" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="O40" s="11" t="s">
+      <c r="O40" s="45" t="s">
         <v>43</v>
       </c>
       <c r="P40" s="1" t="s">
@@ -2137,12 +2536,10 @@
       <c r="Q40" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="R40" s="8"/>
-      <c r="S40" s="6"/>
-      <c r="T40" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="U40" s="10"/>
+      <c r="R40" s="43"/>
+      <c r="S40" s="48"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="56"/>
       <c r="V40" s="2"/>
       <c r="W40" s="2"/>
       <c r="X40" s="2"/>
@@ -2150,44 +2547,44 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:25" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="6"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
-      <c r="E41" s="17" t="s">
+      <c r="E41" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="F41" s="17"/>
-      <c r="G41" s="20" t="s">
+      <c r="F41" s="22"/>
+      <c r="G41" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H41" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="I41" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="J41" s="2"/>
+      <c r="K41" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="H41" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="I41" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="J41" s="2"/>
-      <c r="K41" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="L41" s="17"/>
-      <c r="M41" s="17"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="22"/>
       <c r="N41" s="4"/>
-      <c r="O41" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="P41" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q41" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="R41" s="2"/>
-      <c r="S41" s="2"/>
-      <c r="T41" s="1"/>
-      <c r="U41" s="10"/>
+      <c r="O41" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="P41" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q41" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="R41" s="43"/>
+      <c r="S41" s="48"/>
+      <c r="T41" s="2"/>
+      <c r="U41" s="56"/>
       <c r="V41" s="2"/>
       <c r="W41" s="2"/>
       <c r="X41" s="2"/>
@@ -2195,7 +2592,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:25" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="6" t="s">
         <v>34</v>
       </c>
@@ -2208,10 +2605,10 @@
       <c r="D42" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F42" s="19" t="s">
         <v>1</v>
       </c>
       <c r="G42" s="1" t="s">
@@ -2226,19 +2623,19 @@
       <c r="J42" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K42" s="1" t="s">
+      <c r="K42" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="L42" s="1" t="s">
+      <c r="L42" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="M42" s="1" t="s">
+      <c r="M42" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="N42" s="1" t="s">
+      <c r="N42" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="O42" s="3" t="s">
+      <c r="O42" s="49" t="s">
         <v>10</v>
       </c>
       <c r="P42" s="1" t="s">
@@ -2250,13 +2647,13 @@
       <c r="R42" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="S42" s="1" t="s">
+      <c r="S42" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="T42" s="1" t="s">
+      <c r="T42" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="U42" s="10"/>
+      <c r="U42" s="56"/>
       <c r="V42" s="2"/>
       <c r="W42" s="2"/>
       <c r="X42" s="2"/>
@@ -2264,7 +2661,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:25" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2285,17 +2682,17 @@
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
-      <c r="O43" s="2" t="s">
+      <c r="O43" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="P43" s="2" t="s">
+      <c r="P43" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="Q43" s="2"/>
-      <c r="R43" s="2"/>
-      <c r="S43" s="2"/>
+      <c r="Q43" s="43"/>
+      <c r="R43" s="43"/>
+      <c r="S43" s="48"/>
       <c r="T43" s="2"/>
-      <c r="U43" s="10"/>
+      <c r="U43" s="56"/>
       <c r="V43" s="2"/>
       <c r="W43" s="2"/>
       <c r="X43" s="2"/>
@@ -2303,7 +2700,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:25" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2318,13 +2715,17 @@
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
-      <c r="O44" s="2"/>
-      <c r="P44" s="2"/>
-      <c r="Q44" s="2"/>
-      <c r="R44" s="2"/>
-      <c r="S44" s="2"/>
+      <c r="O44" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="P44" s="51"/>
+      <c r="Q44" s="51"/>
+      <c r="R44" s="51"/>
+      <c r="S44" s="57" t="s">
+        <v>63</v>
+      </c>
       <c r="T44" s="2"/>
-      <c r="U44" s="10"/>
+      <c r="U44" s="56"/>
       <c r="V44" s="2"/>
       <c r="W44" s="2"/>
       <c r="X44" s="2"/>
@@ -2332,7 +2733,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:25" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2347,13 +2748,15 @@
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
-      <c r="O45" s="2"/>
+      <c r="O45" s="9">
+        <v>5</v>
+      </c>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>
-      <c r="S45" s="2"/>
+      <c r="S45" s="53"/>
       <c r="T45" s="2"/>
-      <c r="U45" s="10"/>
+      <c r="U45" s="56"/>
       <c r="V45" s="2"/>
       <c r="W45" s="2"/>
       <c r="X45" s="2"/>
@@ -2361,7 +2764,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:25" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2384,13 +2787,13 @@
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
-      <c r="O46" s="2"/>
-      <c r="P46" s="2"/>
-      <c r="Q46" s="2"/>
-      <c r="R46" s="10"/>
-      <c r="S46" s="10"/>
-      <c r="T46" s="10"/>
-      <c r="U46" s="10"/>
+      <c r="O46" s="9"/>
+      <c r="P46" s="9"/>
+      <c r="Q46" s="9"/>
+      <c r="R46" s="9"/>
+      <c r="S46" s="53"/>
+      <c r="T46" s="56"/>
+      <c r="U46" s="56"/>
       <c r="V46" s="2"/>
       <c r="W46" s="2"/>
       <c r="X46" s="2"/>
@@ -2398,7 +2801,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:25" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2416,8 +2819,8 @@
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
-      <c r="R47" s="10"/>
-      <c r="S47" s="2"/>
+      <c r="R47" s="9"/>
+      <c r="S47" s="53"/>
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
       <c r="V47" s="2"/>
@@ -2427,7 +2830,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:25" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
         <v>16</v>
       </c>
@@ -2467,22 +2870,22 @@
       <c r="M48" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N48" s="1" t="s">
+      <c r="N48" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="O48" s="1" t="s">
+      <c r="O48" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="P48" s="1" t="s">
+      <c r="P48" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="Q48" s="1" t="s">
+      <c r="Q48" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="R48" s="10" t="s">
+      <c r="R48" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="S48" s="1" t="s">
+      <c r="S48" s="6" t="s">
         <v>34</v>
       </c>
       <c r="T48" s="1">
@@ -2496,16 +2899,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:26" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
@@ -2514,17 +2917,17 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
-      <c r="N49" s="21" t="s">
+      <c r="N49" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="O49" s="21" t="s">
+      <c r="O49" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="P49" s="21" t="s">
+      <c r="P49" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="Q49" s="2"/>
-      <c r="R49" s="2"/>
+      <c r="Q49" s="58"/>
+      <c r="R49" s="59"/>
       <c r="S49" s="2"/>
       <c r="T49" s="2"/>
       <c r="U49" s="2"/>
@@ -2535,7 +2938,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:25" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:26" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2549,17 +2952,21 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
-      <c r="N50" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="O50" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="P50" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q50" s="2"/>
-      <c r="R50" s="2"/>
+      <c r="N50" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="O50" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="P50" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q50" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="R50" s="12" t="s">
+        <v>61</v>
+      </c>
       <c r="S50" s="2"/>
       <c r="T50" s="2"/>
       <c r="U50" s="2"/>
@@ -2569,17 +2976,22 @@
       <c r="Y50">
         <v>18</v>
       </c>
+      <c r="Z50">
+        <f>Y50*2.54</f>
+        <v>45.72</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="I14:J14"/>
     <mergeCell ref="P14:R14"/>
     <mergeCell ref="P23:S23"/>
     <mergeCell ref="H23:K23"/>
     <mergeCell ref="D34:G34"/>
     <mergeCell ref="L34:O34"/>
-    <mergeCell ref="K41:M41"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="A30:F30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>